<commit_message>
new memory planning part reviewed
</commit_message>
<xml_diff>
--- a/_memoria/Introducció/projectPlanning.xlsx
+++ b/_memoria/Introducció/projectPlanning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Primer estudi superficial de l'API</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>FASE DEL PROJECTE / MES</t>
+  </si>
+  <si>
+    <t>Preparació de la defensa del projecte</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -963,7 +966,7 @@
     </row>
     <row r="8" spans="1:29" ht="33" customHeight="1">
       <c r="A8" s="19" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>

</xml_diff>